<commit_message>
Add updated evaluation results + initial version sentence transformers learning
</commit_message>
<xml_diff>
--- a/data/results_data_augmention.xlsx
+++ b/data/results_data_augmention.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">RougeSum</t>
   </si>
   <si>
-    <t xml:space="preserve">Score</t>
+    <t xml:space="preserve">score</t>
   </si>
   <si>
     <t xml:space="preserve">std_dev</t>
@@ -46,10 +46,10 @@
     <t xml:space="preserve">Baseline</t>
   </si>
   <si>
-    <t xml:space="preserve">HunFlair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MESH</t>
+    <t xml:space="preserve">HunFlair (1.030)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMLS (1.375)</t>
   </si>
 </sst>
 </file>
@@ -65,6 +65,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -86,6 +87,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,7 +174,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,7 +195,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -214,10 +216,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,10 +239,10 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
@@ -282,7 +280,7 @@
       <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -294,7 +292,7 @@
       <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -364,28 +362,28 @@
         <v>9</v>
       </c>
       <c r="B6" s="9" t="n">
-        <v>51.22485</v>
+        <v>51.39328</v>
       </c>
       <c r="C6" s="10" t="n">
-        <v>2.55820423041242</v>
-      </c>
-      <c r="D6" s="11" t="n">
-        <v>33.2375</v>
-      </c>
-      <c r="E6" s="11" t="n">
-        <v>2.35634102413042</v>
+        <v>2.65853227770513</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>33.45576</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>2.79199697356569</v>
       </c>
       <c r="F6" s="9" t="n">
-        <v>48.08512</v>
+        <v>48.2352</v>
       </c>
       <c r="G6" s="10" t="n">
-        <v>2.72258414518266</v>
-      </c>
-      <c r="H6" s="11" t="n">
-        <v>48.19827</v>
-      </c>
-      <c r="I6" s="11" t="n">
-        <v>2.71882092019684</v>
+        <v>2.86973771379895</v>
+      </c>
+      <c r="H6" s="9" t="n">
+        <v>48.22435</v>
+      </c>
+      <c r="I6" s="10" t="n">
+        <v>2.82599274140964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add updated evaluation results, sent_transformer implementation  and run_cv scripts
</commit_message>
<xml_diff>
--- a/data/results_data_augmention.xlsx
+++ b/data/results_data_augmention.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t xml:space="preserve">Modell</t>
   </si>
@@ -50,15 +50,28 @@
   </si>
   <si>
     <t xml:space="preserve">UMLS (1.375)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard (1.157)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All (14.241)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline (25 Epochs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMLS(25 Epochs)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -174,7 +187,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -216,6 +229,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -236,13 +261,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
@@ -384,6 +409,122 @@
       </c>
       <c r="I6" s="10" t="n">
         <v>2.82599274140964</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>50.90068</v>
+      </c>
+      <c r="C7" s="12" t="n">
+        <v>2.85786775194375</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>33.0555</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>3.17446082414006</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>48.07698</v>
+      </c>
+      <c r="G7" s="12" t="n">
+        <v>3.06952203276015</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>48.1031</v>
+      </c>
+      <c r="I7" s="12" t="n">
+        <v>3.03572142858992</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9" t="n">
+        <v>50.09508</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>2.52975452318995</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>31.87673</v>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>2.79626696938972</v>
+      </c>
+      <c r="F8" s="9" t="n">
+        <v>47.05861</v>
+      </c>
+      <c r="G8" s="10" t="n">
+        <v>2.7852317499447</v>
+      </c>
+      <c r="H8" s="9" t="n">
+        <v>47.05125</v>
+      </c>
+      <c r="I8" s="10" t="n">
+        <v>2.72576951969531</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="9" t="n">
+        <v>51.73345</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>3.11462853106113</v>
+      </c>
+      <c r="D10" s="13" t="n">
+        <v>32.9474</v>
+      </c>
+      <c r="E10" s="13" t="n">
+        <v>2.91815712222629</v>
+      </c>
+      <c r="F10" s="9" t="n">
+        <v>48.23627</v>
+      </c>
+      <c r="G10" s="10" t="n">
+        <v>2.92610029050612</v>
+      </c>
+      <c r="H10" s="9" t="n">
+        <v>48.2129</v>
+      </c>
+      <c r="I10" s="10" t="n">
+        <v>2.98457760260979</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="11" t="n">
+        <v>51.70711</v>
+      </c>
+      <c r="C11" s="12" t="n">
+        <v>3.505571208933</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>33.15246</v>
+      </c>
+      <c r="E11" s="12" t="n">
+        <v>3.26407150938824</v>
+      </c>
+      <c r="F11" s="11" t="n">
+        <v>48.16164</v>
+      </c>
+      <c r="G11" s="12" t="n">
+        <v>3.56640800363615</v>
+      </c>
+      <c r="H11" s="11" t="n">
+        <v>48.21447</v>
+      </c>
+      <c r="I11" s="12" t="n">
+        <v>3.54904576894973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update results for data augments experiments
</commit_message>
<xml_diff>
--- a/data/results_data_augmention.xlsx
+++ b/data/results_data_augmention.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="10_Epochen" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="splits_s777" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="splits_s17" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t xml:space="preserve">Modell</t>
   </si>
@@ -62,16 +63,20 @@
   </si>
   <si>
     <t xml:space="preserve">UMLS(25 Epochs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMLS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -187,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,6 +246,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -263,17 +272,17 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.82"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,4 +552,141 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="n">
+        <v>51.96418</v>
+      </c>
+      <c r="C3" s="14" t="n">
+        <v>2.77187878010565</v>
+      </c>
+      <c r="D3" s="14" t="n">
+        <v>33.12591</v>
+      </c>
+      <c r="E3" s="14" t="n">
+        <v>2.86646037176515</v>
+      </c>
+      <c r="F3" s="14" t="n">
+        <v>48.5848</v>
+      </c>
+      <c r="G3" s="14" t="n">
+        <v>2.79456900362113</v>
+      </c>
+      <c r="H3" s="14" t="n">
+        <v>48.57656</v>
+      </c>
+      <c r="I3" s="14" t="n">
+        <v>2.70610107098756</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="13" t="n">
+        <v>50.61776</v>
+      </c>
+      <c r="C5" s="13" t="n">
+        <v>2.85417294787825</v>
+      </c>
+      <c r="D5" s="13" t="n">
+        <v>31.88127</v>
+      </c>
+      <c r="E5" s="13" t="n">
+        <v>3.13389577013978</v>
+      </c>
+      <c r="F5" s="13" t="n">
+        <v>47.29161</v>
+      </c>
+      <c r="G5" s="13" t="n">
+        <v>3.1328959904376</v>
+      </c>
+      <c r="H5" s="13" t="n">
+        <v>47.32887</v>
+      </c>
+      <c r="I5" s="13" t="n">
+        <v>3.05178670160613</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>